<commit_message>
update bom and add desc
Signed-off-by: YuzukiTsuru <gloomyghist@gloomyghost.com>
</commit_message>
<xml_diff>
--- a/Hardware/BOM&PickAndPlace/BOM_Board1_PCB1_2022-08-28.xlsx
+++ b/Hardware/BOM&PickAndPlace/BOM_Board1_PCB1_2022-08-28.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Board1_PCB1_2022-08-28" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="214">
   <si>
     <t>Device</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Manufacturer Part</t>
+  </si>
+  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -31,9 +34,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>Manufacturer Part</t>
-  </si>
-  <si>
     <t>Supplier Part (LCSC)</t>
   </si>
   <si>
@@ -52,9 +52,6 @@
     <t>BGA284P65B1200_1400H125</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -70,7 +67,7 @@
     <t>FBGA96</t>
   </si>
   <si>
-    <t>You can choose compatible DDR3 and DDR3L memory, up to 2GB</t>
+    <t>可选择单 Rank 或双 Rank 的 DDR3、DDR3L 内存颗粒</t>
   </si>
   <si>
     <t>AXP1530</t>
@@ -85,6 +82,9 @@
     <t>WQFN-20_L3.0-W3.0-P0.40-BL-EP</t>
   </si>
   <si>
+    <t>H616 的 配套PMIC</t>
+  </si>
+  <si>
     <t>RGBLED_0807</t>
   </si>
   <si>
@@ -97,6 +97,9 @@
     <t>RGB LED</t>
   </si>
   <si>
+    <t>0807 自闪 RGB LED 灯，https://item.taobao.com/item.htm?spm=a1z09.2.0.0.43bd2e8dvLJwkL&amp;id=640536151317&amp;_u=r29eas9a2ab0</t>
+  </si>
+  <si>
     <t>XR829</t>
   </si>
   <si>
@@ -106,6 +109,9 @@
     <t>QFN-40_L5.0-W5.0-P0.40-BL-EP3.4</t>
   </si>
   <si>
+    <t>XR829 WIFI</t>
+  </si>
+  <si>
     <t>B-2100S40P-B110</t>
   </si>
   <si>
@@ -124,15 +130,15 @@
     <t>THGBMJG7C1LBAIL</t>
   </si>
   <si>
+    <t>EMMC04G-M627-A01</t>
+  </si>
+  <si>
     <t>U4</t>
   </si>
   <si>
     <t>FBGA-153_L13.0-W11.5</t>
   </si>
   <si>
-    <t>EMMC04G-M627-A01</t>
-  </si>
-  <si>
     <t>C879825</t>
   </si>
   <si>
@@ -151,22 +157,28 @@
     <t>C40960</t>
   </si>
   <si>
-    <t>Optional</t>
+    <t>ESD组件，测试可不贴</t>
   </si>
   <si>
     <t>MLP2016S1R0MT0S1</t>
   </si>
   <si>
+    <t>1239AS-H-1R0M=P2</t>
+  </si>
+  <si>
+    <t>L1,L2,L3</t>
+  </si>
+  <si>
     <t>1uH</t>
   </si>
   <si>
-    <t>L1,L2,L3</t>
-  </si>
-  <si>
-    <t>IND-SMD_L2.0-W1.6_1</t>
-  </si>
-  <si>
-    <t>C76793</t>
+    <t>IND-SMD_L2.5-W2.0</t>
+  </si>
+  <si>
+    <t>C167447</t>
+  </si>
+  <si>
+    <t>1uH，2520 封装电感，饱和 2.5A 以上</t>
   </si>
   <si>
     <t>HDMI-019S</t>
@@ -181,18 +193,24 @@
     <t>C111617</t>
   </si>
   <si>
+    <t>HDMI 接口</t>
+  </si>
+  <si>
+    <t>1040310811</t>
+  </si>
+  <si>
     <t>SIM1</t>
   </si>
   <si>
     <t>SIM-SMD_8P-1040310811</t>
   </si>
   <si>
-    <t>1040310811</t>
-  </si>
-  <si>
     <t>C585350</t>
   </si>
   <si>
+    <t>TF 卡槽</t>
+  </si>
+  <si>
     <t>U.FL-R-SMT-1(80)</t>
   </si>
   <si>
@@ -205,19 +223,25 @@
     <t>C88374</t>
   </si>
   <si>
+    <t>WIFI 天线</t>
+  </si>
+  <si>
+    <t>0533980271</t>
+  </si>
+  <si>
     <t>FAN1</t>
   </si>
   <si>
     <t>CONN-SMD_2P-P1.25_053398-0X71</t>
   </si>
   <si>
-    <t>0533980271</t>
-  </si>
-  <si>
     <t>C122410</t>
   </si>
   <si>
-    <t>BAS516,115</t>
+    <t>风扇接口</t>
+  </si>
+  <si>
+    <t>RB521S-30</t>
   </si>
   <si>
     <t>D20</t>
@@ -226,9 +250,6 @@
     <t>SOD-523_L1.2-W0.8-LS1.6-FD</t>
   </si>
   <si>
-    <t>1N5819-SOD523</t>
-  </si>
-  <si>
     <t>C122862</t>
   </si>
   <si>
@@ -277,7 +298,7 @@
     <t>D1,D22,D23</t>
   </si>
   <si>
-    <t>SOD-323_L1.8-W1.3-LS2.5-NSK</t>
+    <t>SOD-323_L1.8-W1.3-LS2.5</t>
   </si>
   <si>
     <t>C248733</t>
@@ -331,88 +352,184 @@
     <t>C165948</t>
   </si>
   <si>
+    <t>0402WGF0000TCE</t>
+  </si>
+  <si>
     <t>Res_0402</t>
   </si>
   <si>
+    <t>R4,R5,R18,R32</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>C17168</t>
+  </si>
+  <si>
+    <t>0402WGF220JTCE</t>
+  </si>
+  <si>
+    <t>R27,R29</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>C25092</t>
+  </si>
+  <si>
+    <t>0402WGF330JTCE</t>
+  </si>
+  <si>
+    <t>R12,R13,R14</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>C25105</t>
+  </si>
+  <si>
+    <t>0402WGF750JTCE</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>C25133</t>
+  </si>
+  <si>
+    <t>0402WGF1000TCE</t>
+  </si>
+  <si>
+    <t>R7,R38,R42,R45</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>C25076</t>
+  </si>
+  <si>
+    <t>RC0402FR-07240RL</t>
+  </si>
+  <si>
+    <t>R6,R8,R9</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>C114755</t>
+  </si>
+  <si>
+    <t>DRAM ZQ校准电阻，1%精度</t>
+  </si>
+  <si>
+    <t>0402WGF5100TCE</t>
+  </si>
+  <si>
+    <t>R1,R28</t>
+  </si>
+  <si>
+    <t>C25123</t>
+  </si>
+  <si>
+    <t>0402WGF1001TCE</t>
+  </si>
+  <si>
+    <t>R15,R34,R39</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>C11702</t>
+  </si>
+  <si>
+    <t>0402WGF2001TCE</t>
+  </si>
+  <si>
+    <t>R10,R11</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>C4109</t>
+  </si>
+  <si>
+    <t>0402WGF5101TCE</t>
+  </si>
+  <si>
+    <t>R35,R36,R40,R43,R44,R46,R48</t>
+  </si>
+  <si>
+    <t>5.1K</t>
+  </si>
+  <si>
+    <t>C25905</t>
+  </si>
+  <si>
+    <t>RC-02W6041FT</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>6.04k</t>
+  </si>
+  <si>
+    <t>C304624</t>
+  </si>
+  <si>
+    <t>内置PHY耦合电阻，1%精度</t>
+  </si>
+  <si>
+    <t>0402WGF1002TCE</t>
+  </si>
+  <si>
     <t>R2,R3,R41,R47,R49</t>
   </si>
   <si>
     <t>10K</t>
   </si>
   <si>
-    <t>R0402</t>
-  </si>
-  <si>
     <t>C25744</t>
   </si>
   <si>
-    <t>R27,R29</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>C25092</t>
-  </si>
-  <si>
-    <t>R1,R28</t>
-  </si>
-  <si>
-    <t>C25123</t>
-  </si>
-  <si>
-    <t>R4,R5,R18,R32</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>C17168</t>
+    <t>0402WGF2702TCE</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>27K</t>
+  </si>
+  <si>
+    <t>C25771</t>
+  </si>
+  <si>
+    <t>0402WGF4702TCE</t>
   </si>
   <si>
     <t>R33,R16,R17,R19,R20,R21,R22,R23,R24,R25</t>
   </si>
   <si>
-    <t>47k</t>
+    <t>47K</t>
   </si>
   <si>
     <t>C25792</t>
   </si>
   <si>
-    <t>R15,R34</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>C11702</t>
-  </si>
-  <si>
-    <t>R35,R36,R40,R43,R44,R46,R48</t>
-  </si>
-  <si>
-    <t>5.1k</t>
-  </si>
-  <si>
-    <t>C25905</t>
-  </si>
-  <si>
-    <t>R7,R38,R42,R45</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>C25076</t>
-  </si>
-  <si>
-    <t>R12,R13,R14</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>C25105</t>
+    <t>RC0402FR-07150KL</t>
   </si>
   <si>
     <t>R31</t>
@@ -424,145 +541,121 @@
     <t>C93947</t>
   </si>
   <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
-    <t>27K</t>
-  </si>
-  <si>
-    <t>C25771</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>C25133</t>
-  </si>
-  <si>
-    <t>R6,R8,R9</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>C114755</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>6.04k</t>
-  </si>
-  <si>
-    <t>C304624</t>
-  </si>
-  <si>
-    <t>R10,R11</t>
-  </si>
-  <si>
-    <t>2k</t>
-  </si>
-  <si>
-    <t>C4109</t>
+    <t>0402CG220J500NT</t>
   </si>
   <si>
     <t>CAP_0402</t>
   </si>
   <si>
+    <t>C80,C85,C94,C99</t>
+  </si>
+  <si>
+    <t>22pF</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>C1555</t>
+  </si>
+  <si>
+    <t>CL05B104KO5NNNC</t>
+  </si>
+  <si>
     <t>C14,C15,C16,C17,C18,C19,C20,C21,C22,C23,C24,C25,C26,C27,C28,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C39,C40,C41,C42,C43,C44,C45,C46,C47,C48,C49,C50,C51,C52,C53,C54,C55,C56,C57,C58,C59,C60,C61,C62,C63,C64,C65,C88,C90,C86,C87,C98,C100</t>
   </si>
   <si>
     <t>100nF</t>
   </si>
   <si>
-    <t>C0402</t>
-  </si>
-  <si>
     <t>C1525</t>
   </si>
   <si>
+    <t>CL05B224KO5NNNC</t>
+  </si>
+  <si>
+    <t>C97</t>
+  </si>
+  <si>
+    <t>220nF</t>
+  </si>
+  <si>
+    <t>C16772</t>
+  </si>
+  <si>
+    <t>CL05A474KP5NNNC</t>
+  </si>
+  <si>
+    <t>C92,C93</t>
+  </si>
+  <si>
+    <t>470nF</t>
+  </si>
+  <si>
+    <t>C47339</t>
+  </si>
+  <si>
+    <t>CL05A105KA5NQNC</t>
+  </si>
+  <si>
+    <t>C12,C68,C69,C70,C71,C72,C73,C74,C78,C79,C84,C96</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>C52923</t>
+  </si>
+  <si>
+    <t>CL05A225MQ5NSNC</t>
+  </si>
+  <si>
+    <t>C75,C76,C77,C81,C82,C83,C95</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>C12530</t>
+  </si>
+  <si>
+    <t>CL05A475MP5NRNC</t>
+  </si>
+  <si>
     <t>C1,C3,C5,C89,C91</t>
   </si>
   <si>
-    <t>4.7uf</t>
+    <t>4.7uF</t>
   </si>
   <si>
     <t>C23733</t>
   </si>
   <si>
-    <t>C12,C68,C69,C70,C71,C72,C73,C74,C78,C79,C84,C96</t>
-  </si>
-  <si>
-    <t>1uf</t>
-  </si>
-  <si>
-    <t>C52923</t>
-  </si>
-  <si>
-    <t>C75,C76,C77,C81,C82,C83,C95</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>C12530</t>
-  </si>
-  <si>
-    <t>C97</t>
-  </si>
-  <si>
-    <t>220nF</t>
-  </si>
-  <si>
-    <t>C16772</t>
-  </si>
-  <si>
-    <t>C92,C93</t>
-  </si>
-  <si>
-    <t>470nF</t>
-  </si>
-  <si>
-    <t>C47339</t>
-  </si>
-  <si>
-    <t>C80,C85,C94,C99</t>
-  </si>
-  <si>
-    <t>22pf</t>
-  </si>
-  <si>
-    <t>C1555</t>
+    <t>CL10A475KO8NNNC</t>
   </si>
   <si>
     <t>CAP_0603</t>
   </si>
   <si>
+    <t>C2,C7,C10</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>C19666</t>
+  </si>
+  <si>
+    <t>CL10A226MQ8NRNC</t>
+  </si>
+  <si>
     <t>C4,C6,C8,C9,C11,C13</t>
   </si>
   <si>
-    <t>22uf</t>
-  </si>
-  <si>
-    <t>C0603</t>
+    <t>22uF</t>
   </si>
   <si>
     <t>C59461</t>
-  </si>
-  <si>
-    <t>C2,C7,C10</t>
-  </si>
-  <si>
-    <t>C19666</t>
   </si>
 </sst>
 </file>
@@ -575,14 +668,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1038,48 +1124,51 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1089,100 +1178,97 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1571,22 +1657,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="61.1416666666667" customWidth="1"/>
-    <col min="4" max="4" width="21.8583333333333" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.8583333333333" customWidth="1"/>
-    <col min="6" max="6" width="21.8583333333333" customWidth="1"/>
-    <col min="7" max="7" width="12.7083333333333" customWidth="1"/>
-    <col min="8" max="8" width="61.425" customWidth="1"/>
+    <col min="3" max="3" width="21.8583333333333" customWidth="1"/>
+    <col min="4" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="21.8583333333333" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.8583333333333" customWidth="1"/>
+    <col min="7" max="7" width="27.625" customWidth="1"/>
+    <col min="8" max="8" width="83.5" customWidth="1"/>
+    <col min="9" max="9" width="43.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1623,71 +1710,75 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
@@ -1696,172 +1787,178 @@
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1">
@@ -1871,835 +1968,871 @@
         <v>1040310811</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="1">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1">
         <v>1040310811</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>533980271</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="1">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="1">
         <v>533980271</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B23" s="1"/>
+        <v>108</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G25" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D26" s="1">
-        <v>510</v>
+        <v>122</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G26" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>132</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H29" s="1"/>
+      <c r="A29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" t="s">
+        <v>137</v>
+      </c>
+      <c r="H29" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E30" s="1">
+        <v>510</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G30" s="1" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F31" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G31" s="1" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>105</v>
+        <v>146</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G32" s="1" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G33" s="1" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H34" s="1"/>
+      <c r="A34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s">
+        <v>154</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" t="s">
+        <v>156</v>
+      </c>
+      <c r="F34" t="s">
+        <v>116</v>
+      </c>
+      <c r="G34" t="s">
+        <v>157</v>
+      </c>
+      <c r="H34" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G35" s="1" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>163</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G36" s="1" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" t="s">
-        <v>108</v>
-      </c>
-      <c r="F37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>105</v>
-      </c>
-      <c r="B38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" t="s">
-        <v>149</v>
-      </c>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>105</v>
+        <v>176</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>178</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="G39" s="1" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F40" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="G40" s="1" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>187</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="G41" s="1" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="G42" s="1" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F43" s="1"/>
+        <v>195</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="G43" s="1" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>199</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="G44" s="1" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>203</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>179</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>153</v>
+        <v>206</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F46" s="1"/>
+        <v>203</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="G46" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F47" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="G47" s="1" t="s">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H48" s="1"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>

</xml_diff>